<commit_message>
added target indicator for Stick-BOT
</commit_message>
<xml_diff>
--- a/doc.xlsx
+++ b/doc.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Breakout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\Breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -564,23 +564,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" style="4" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="41.85546875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="41.81640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -603,7 +603,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -620,7 +620,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -628,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>303</v>
+        <v>375</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -646,12 +646,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -669,12 +669,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="1">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -692,20 +692,20 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>472</v>
+        <v>493</v>
       </c>
       <c r="D6" s="1">
         <f>SUM(C3:C6)</f>
-        <v>1011</v>
+        <v>1136</v>
       </c>
       <c r="E6" s="1">
         <f>SUM(D3:D6)</f>
-        <v>1011</v>
+        <v>1136</v>
       </c>
       <c r="G6" s="2">
         <v>42828</v>
@@ -721,7 +721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -739,7 +739,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>55</v>
       </c>
@@ -765,7 +765,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>53</v>
       </c>
@@ -788,7 +788,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>54</v>
       </c>
@@ -801,7 +801,7 @@
       </c>
       <c r="E10" s="1">
         <f>SUM(D3:D10)</f>
-        <v>1099</v>
+        <v>1224</v>
       </c>
       <c r="G10" s="2">
         <v>42842</v>
@@ -817,16 +817,20 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G11" s="2"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G11" s="2">
+        <v>42984</v>
+      </c>
       <c r="H11" s="3">
         <f>I11-I10</f>
-        <v>-5413</v>
-      </c>
-      <c r="I11" s="3"/>
+        <v>239</v>
+      </c>
+      <c r="I11" s="3">
+        <v>5652</v>
+      </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>49</v>
       </c>
@@ -834,24 +838,24 @@
         <v>48</v>
       </c>
       <c r="C12" s="1">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D12" s="1">
         <f>SUM(C12:C12)</f>
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E12" s="1">
         <f>SUM(D7:D12)</f>
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="3">
         <f>I12-I11</f>
-        <v>0</v>
+        <v>-5652</v>
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -862,7 +866,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
@@ -870,7 +874,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -879,20 +883,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D15" s="1">
         <f>SUM(C14:C15)</f>
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E15" s="1">
         <f>SUM(D3:D15)</f>
-        <v>1481</v>
+        <v>1606</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3">
@@ -902,7 +906,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -914,7 +918,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -922,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -934,12 +938,12 @@
       <c r="I17" s="3"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1">
-        <v>416</v>
+        <v>462</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -951,12 +955,12 @@
       <c r="I18" s="3"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="1">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -968,12 +972,12 @@
       <c r="I19" s="3"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="1">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -985,12 +989,12 @@
       <c r="I20" s="3"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1002,12 +1006,12 @@
       <c r="I21" s="3"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="1">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1019,12 +1023,12 @@
       <c r="I22" s="3"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="1">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1036,12 +1040,12 @@
       <c r="I23" s="3"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B24" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="1">
-        <v>252</v>
+        <v>286</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1053,12 +1057,12 @@
       <c r="I24" s="3"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B25" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="1">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1070,12 +1074,12 @@
       <c r="I25" s="3"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="1">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1087,7 +1091,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B27" s="4" t="s">
         <v>18</v>
       </c>
@@ -1096,11 +1100,11 @@
       </c>
       <c r="D27" s="1">
         <f>SUM(C17:C27)</f>
-        <v>1773</v>
+        <v>1882</v>
       </c>
       <c r="E27" s="1">
         <f>SUM(D3:D27)</f>
-        <v>3254</v>
+        <v>3488</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3">
@@ -1110,7 +1114,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1122,7 +1126,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>40</v>
       </c>
@@ -1130,7 +1134,7 @@
         <v>41</v>
       </c>
       <c r="C29" s="1">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1142,7 +1146,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>42</v>
       </c>
@@ -1151,11 +1155,11 @@
       </c>
       <c r="D30" s="1">
         <f>SUM(C29:C30)</f>
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E30" s="1">
         <f>SUM(D3:D30)</f>
-        <v>3548</v>
+        <v>3786</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3">
@@ -1165,7 +1169,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1177,7 +1181,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>3</v>
       </c>
@@ -1185,7 +1189,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="1">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1197,12 +1201,12 @@
       <c r="I32" s="3"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B33" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="1">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1214,12 +1218,12 @@
       <c r="I33" s="3"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="1">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1231,12 +1235,12 @@
       <c r="I34" s="3"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C35" s="1">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1248,7 +1252,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B36" s="4" t="s">
         <v>23</v>
       </c>
@@ -1265,20 +1269,20 @@
       <c r="I36" s="3"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B37" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="1">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D37" s="1">
         <f>SUM(C32:C37)</f>
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="E37" s="1">
         <f>SUM(D3:D37)</f>
-        <v>5084</v>
+        <v>5323</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3">
@@ -1288,7 +1292,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1300,7 +1304,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>28</v>
       </c>
@@ -1316,7 +1320,7 @@
       </c>
       <c r="E39" s="1">
         <f>SUM(D3:D39)</f>
-        <v>5127</v>
+        <v>5366</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3">
@@ -1326,7 +1330,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1338,7 +1342,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>30</v>
       </c>
@@ -1358,7 +1362,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B42" s="4" t="s">
         <v>51</v>
       </c>
@@ -1371,7 +1375,7 @@
       </c>
       <c r="E42" s="1">
         <f>SUM(D3:D42)</f>
-        <v>5413</v>
+        <v>5652</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3">
@@ -1381,13 +1385,13 @@
       <c r="I42" s="3"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>

</xml_diff>

<commit_message>
removed unused image files
</commit_message>
<xml_diff>
--- a/doc.xlsx
+++ b/doc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>engine.entity</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>highscore and options cleanup</t>
+  </si>
+  <si>
+    <t>added target indicator for Stick-BOT</t>
   </si>
 </sst>
 </file>
@@ -567,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,7 +831,9 @@
       <c r="I11" s="3">
         <v>5652</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">

</xml_diff>